<commit_message>
Änderung der Werte in der Spalte IT-Ausstatung
Änderung von (Ja/Nein) ind (J/N)
</commit_message>
<xml_diff>
--- a/Doku/Stammdaten_Datenbank.xlsx
+++ b/Doku/Stammdaten_Datenbank.xlsx
@@ -199,12 +199,6 @@
     <t>IT-Ausstatung</t>
   </si>
   <si>
-    <t>JA</t>
-  </si>
-  <si>
-    <t>NEIN</t>
-  </si>
-  <si>
     <t>cf101</t>
   </si>
   <si>
@@ -266,6 +260,12 @@
   </si>
   <si>
     <t>BABM3</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -782,8 +782,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -808,7 +810,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -833,7 +834,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="77">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -871,6 +872,7 @@
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -908,6 +910,7 @@
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1239,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1255,12 +1258,12 @@
     <col min="10" max="10" width="5" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="46" customFormat="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" s="45" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="46" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="45" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1275,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="22"/>
-      <c r="H3" s="33"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="23"/>
       <c r="L3" s="2" t="s">
         <v>32</v>
@@ -1286,26 +1289,26 @@
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="16"/>
-      <c r="F4" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="44" t="s">
+      <c r="H4" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="43" t="s">
         <v>58</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="40" t="s">
+      <c r="B5" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="16"/>
@@ -1318,14 +1321,14 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="40" t="s">
-        <v>74</v>
+      <c r="I5" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="N5" s="16"/>
     </row>
@@ -1334,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="16"/>
       <c r="F6" s="4">
@@ -1343,11 +1346,11 @@
       <c r="G6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="30">
         <v>2</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="L6" s="21">
         <v>1</v>
@@ -1362,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" s="16"/>
       <c r="F7" s="4">
@@ -1371,11 +1374,11 @@
       <c r="G7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <v>3</v>
       </c>
-      <c r="I7" s="26" t="s">
-        <v>60</v>
+      <c r="I7" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L7" s="21">
         <v>1</v>
@@ -1390,7 +1393,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1398,11 +1401,11 @@
       <c r="G8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="30">
         <v>4</v>
       </c>
-      <c r="I8" s="26" t="s">
-        <v>60</v>
+      <c r="I8" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L8" s="21">
         <v>1</v>
@@ -1417,7 +1420,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
@@ -1425,11 +1428,11 @@
       <c r="G9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="30">
         <v>5</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>60</v>
+      <c r="I9" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L9" s="21">
         <v>1</v>
@@ -1440,11 +1443,11 @@
       <c r="N9" s="16"/>
     </row>
     <row r="10" spans="1:14" ht="18">
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" s="4">
         <v>6</v>
@@ -1452,11 +1455,11 @@
       <c r="G10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="30">
         <v>6</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>60</v>
+      <c r="I10" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L10" s="21">
         <v>1</v>
@@ -1471,7 +1474,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4">
         <v>7</v>
@@ -1479,11 +1482,11 @@
       <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="30">
         <v>3</v>
       </c>
-      <c r="I11" s="26" t="s">
-        <v>59</v>
+      <c r="I11" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L11" s="21">
         <v>1</v>
@@ -1494,19 +1497,19 @@
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="F12" s="4">
         <v>8</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="30">
         <v>2</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>59</v>
+      <c r="I12" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L12" s="21">
         <v>2</v>
@@ -1525,11 +1528,11 @@
       <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="30">
         <v>9</v>
       </c>
-      <c r="I13" s="26" t="s">
-        <v>60</v>
+      <c r="I13" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L13" s="21">
         <v>2</v>
@@ -1548,11 +1551,11 @@
       <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="30">
         <v>9</v>
       </c>
-      <c r="I14" s="26" t="s">
-        <v>60</v>
+      <c r="I14" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L14" s="21">
         <v>2</v>
@@ -1569,11 +1572,11 @@
       <c r="G15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="30">
         <v>2</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>59</v>
+      <c r="I15" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L15" s="21">
         <v>2</v>
@@ -1590,11 +1593,11 @@
       <c r="G16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="30">
         <v>3</v>
       </c>
-      <c r="I16" s="26" t="s">
-        <v>59</v>
+      <c r="I16" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L16" s="21">
         <v>2</v>
@@ -1611,11 +1614,11 @@
       <c r="G17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="30">
         <v>2</v>
       </c>
-      <c r="I17" s="26" t="s">
-        <v>59</v>
+      <c r="I17" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L17" s="21">
         <v>3</v>
@@ -1629,7 +1632,7 @@
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="16"/>
       <c r="F18" s="4">
         <v>14</v>
@@ -1637,11 +1640,11 @@
       <c r="G18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="30">
         <v>10</v>
       </c>
-      <c r="I18" s="26" t="s">
-        <v>59</v>
+      <c r="I18" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L18" s="21">
         <v>3</v>
@@ -1652,8 +1655,8 @@
       <c r="N18" s="16"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="16"/>
       <c r="F19" s="4">
         <v>15</v>
@@ -1661,11 +1664,11 @@
       <c r="G19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="30">
         <v>9</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>60</v>
+      <c r="I19" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L19" s="21">
         <v>3</v>
@@ -1676,10 +1679,10 @@
       <c r="N19" s="16"/>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="40" t="s">
+      <c r="B20" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="16"/>
@@ -1689,11 +1692,11 @@
       <c r="G20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="30">
         <v>11</v>
       </c>
-      <c r="I20" s="26" t="s">
-        <v>60</v>
+      <c r="I20" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L20" s="21">
         <v>3</v>
@@ -1717,11 +1720,11 @@
       <c r="G21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="31">
+      <c r="H21" s="30">
         <v>8</v>
       </c>
-      <c r="I21" s="26" t="s">
-        <v>60</v>
+      <c r="I21" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L21" s="21">
         <v>3</v>
@@ -1745,11 +1748,11 @@
       <c r="G22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="31">
+      <c r="H22" s="30">
         <v>12</v>
       </c>
-      <c r="I22" s="26" t="s">
-        <v>60</v>
+      <c r="I22" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L22" s="21">
         <v>3</v>
@@ -1773,11 +1776,11 @@
       <c r="G23" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="31">
+      <c r="H23" s="30">
         <v>13</v>
       </c>
-      <c r="I23" s="26" t="s">
-        <v>60</v>
+      <c r="I23" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L23" s="21">
         <v>4</v>
@@ -1801,11 +1804,11 @@
       <c r="G24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="31">
+      <c r="H24" s="30">
         <v>4</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>60</v>
+      <c r="I24" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L24" s="21">
         <v>4</v>
@@ -1829,11 +1832,11 @@
       <c r="G25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="31">
+      <c r="H25" s="30">
         <v>1</v>
       </c>
-      <c r="I25" s="26" t="s">
-        <v>59</v>
+      <c r="I25" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="L25" s="21">
         <v>4</v>
@@ -1857,11 +1860,11 @@
       <c r="G26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="30">
         <v>8</v>
       </c>
-      <c r="I26" s="26" t="s">
-        <v>60</v>
+      <c r="I26" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L26" s="21">
         <v>4</v>
@@ -1885,11 +1888,11 @@
       <c r="G27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="31">
+      <c r="H27" s="30">
         <v>14</v>
       </c>
-      <c r="I27" s="26" t="s">
-        <v>60</v>
+      <c r="I27" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L27" s="21">
         <v>5</v>
@@ -1913,11 +1916,11 @@
       <c r="G28" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="30">
         <v>15</v>
       </c>
-      <c r="I28" s="26" t="s">
-        <v>60</v>
+      <c r="I28" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L28" s="21">
         <v>5</v>
@@ -1941,11 +1944,11 @@
       <c r="G29" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H29" s="30">
         <v>10</v>
       </c>
-      <c r="I29" s="26" t="s">
-        <v>60</v>
+      <c r="I29" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L29" s="21">
         <v>5</v>
@@ -1969,11 +1972,11 @@
       <c r="G30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="30">
         <v>17</v>
       </c>
-      <c r="I30" s="26" t="s">
-        <v>60</v>
+      <c r="I30" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L30" s="21">
         <v>5</v>
@@ -1997,11 +2000,11 @@
       <c r="G31" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="31">
+      <c r="H31" s="30">
         <v>16</v>
       </c>
-      <c r="I31" s="26" t="s">
-        <v>60</v>
+      <c r="I31" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L31" s="21">
         <v>6</v>
@@ -2022,14 +2025,14 @@
       <c r="F32" s="4">
         <v>28</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="34">
+      <c r="H32" s="33">
         <v>18</v>
       </c>
-      <c r="I32" s="26" t="s">
-        <v>60</v>
+      <c r="I32" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L32" s="21">
         <v>6</v>
@@ -2050,14 +2053,14 @@
       <c r="F33" s="4">
         <v>29</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H33" s="33">
         <v>10</v>
       </c>
-      <c r="I33" s="26" t="s">
-        <v>60</v>
+      <c r="I33" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L33" s="21">
         <v>6</v>
@@ -2081,11 +2084,11 @@
       <c r="G34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="31">
+      <c r="H34" s="30">
         <v>7</v>
       </c>
-      <c r="I34" s="26" t="s">
-        <v>60</v>
+      <c r="I34" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="L34" s="21">
         <v>6</v>
@@ -2106,14 +2109,14 @@
       <c r="F35" s="6">
         <v>31</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="34">
         <v>3</v>
       </c>
-      <c r="I35" s="29" t="s">
-        <v>60</v>
+      <c r="I35" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="L35" s="21">
         <v>4</v>
@@ -2189,14 +2192,14 @@
         <v>56</v>
       </c>
       <c r="C41" s="12"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="38"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="37"/>
     </row>
     <row r="42" spans="2:14">
       <c r="B42" s="4"/>
       <c r="C42" s="13"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="38"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="37"/>
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="4" t="s">
@@ -2205,154 +2208,154 @@
       <c r="C43" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="2:14">
       <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="D44" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="2:14">
       <c r="B45" s="4">
         <v>2</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="38"/>
+        <v>60</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="2:14">
       <c r="B46" s="4">
         <v>3</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="38"/>
+        <v>61</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="37"/>
     </row>
     <row r="47" spans="2:14">
       <c r="B47" s="21">
         <v>4</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="38"/>
+        <v>62</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="37"/>
     </row>
     <row r="48" spans="2:14">
       <c r="B48" s="21">
         <v>5</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="38"/>
+        <v>63</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" s="37"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="21">
         <v>6</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49" s="38"/>
+        <v>64</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="37"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="21">
         <v>7</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" s="38"/>
+        <v>65</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="37"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="21">
         <v>8</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="38"/>
+        <v>66</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" s="37"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="21">
         <v>9</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="38"/>
+        <v>67</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="37"/>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="21">
         <v>10</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="38"/>
+        <v>68</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="21">
         <v>11</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="38"/>
+        <v>69</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="2:5" ht="16" thickBot="1">
       <c r="B55" s="15">
         <v>12</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="38"/>
+        <v>70</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="37"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="11"/>

</xml_diff>

<commit_message>
Übernahme der Tabellennamen aus dem SQL-Skript
Tabellennamen wurden aus dem Sql-Strip übernommen
</commit_message>
<xml_diff>
--- a/Doku/Stammdaten_Datenbank.xlsx
+++ b/Doku/Stammdaten_Datenbank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
   <si>
     <t>Studiengang</t>
   </si>
   <si>
-    <t>Module</t>
-  </si>
-  <si>
     <t>IT-Basistechnologien</t>
   </si>
   <si>
@@ -118,15 +115,9 @@
     <t>Wirtschsftsprivatrecht</t>
   </si>
   <si>
-    <t>Studiengangmodule</t>
-  </si>
-  <si>
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>Dozent</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
     <t>Zuordnungstabellen</t>
   </si>
   <si>
-    <t>Raum</t>
-  </si>
-  <si>
     <t>R_ID</t>
   </si>
   <si>
@@ -266,6 +254,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>sp_modul</t>
+  </si>
+  <si>
+    <t>sp_modul_studiengang</t>
+  </si>
+  <si>
+    <t>sp_dozent</t>
+  </si>
+  <si>
+    <t>sp_studiengang</t>
+  </si>
+  <si>
+    <t>sp_raum</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1256,32 +1259,34 @@
     <col min="8" max="8" width="8.33203125" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="5" style="19" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="45" customFormat="1">
       <c r="A1" s="45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J1" s="46"/>
       <c r="K1" s="45" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16" thickBot="1"/>
     <row r="3" spans="1:14" ht="19" thickTop="1">
       <c r="B3" s="9" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="16"/>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="32"/>
       <c r="I3" s="23"/>
       <c r="L3" s="2" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="M3" s="3"/>
     </row>
@@ -1290,23 +1295,23 @@
       <c r="C4" s="8"/>
       <c r="D4" s="16"/>
       <c r="F4" s="38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="42" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" s="38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>0</v>
@@ -1316,19 +1321,19 @@
         <v>1</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L5" s="44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N5" s="16"/>
     </row>
@@ -1337,20 +1342,20 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D6" s="16"/>
       <c r="F6" s="4">
         <v>2</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="30">
         <v>2</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L6" s="21">
         <v>1</v>
@@ -1365,20 +1370,20 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" s="16"/>
       <c r="F7" s="4">
         <v>3</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="30">
         <v>3</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L7" s="21">
         <v>1</v>
@@ -1393,19 +1398,19 @@
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" s="30">
         <v>4</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L8" s="21">
         <v>1</v>
@@ -1420,19 +1425,19 @@
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="30">
         <v>5</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L9" s="21">
         <v>1</v>
@@ -1447,19 +1452,19 @@
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F10" s="4">
         <v>6</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H10" s="30">
         <v>6</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L10" s="21">
         <v>1</v>
@@ -1474,19 +1479,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F11" s="4">
         <v>7</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="30">
         <v>3</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L11" s="21">
         <v>1</v>
@@ -1503,13 +1508,13 @@
         <v>8</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="30">
         <v>2</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L12" s="21">
         <v>2</v>
@@ -1526,13 +1531,13 @@
         <v>9</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" s="30">
         <v>9</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L13" s="21">
         <v>2</v>
@@ -1549,13 +1554,13 @@
         <v>10</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="30">
         <v>9</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L14" s="21">
         <v>2</v>
@@ -1570,13 +1575,13 @@
         <v>11</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="30">
         <v>2</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L15" s="21">
         <v>2</v>
@@ -1591,13 +1596,13 @@
         <v>12</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="30">
         <v>3</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L16" s="21">
         <v>2</v>
@@ -1612,13 +1617,13 @@
         <v>13</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="30">
         <v>2</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L17" s="21">
         <v>3</v>
@@ -1630,7 +1635,7 @@
     </row>
     <row r="18" spans="2:14" ht="18">
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="16"/>
@@ -1638,13 +1643,13 @@
         <v>14</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="30">
         <v>10</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L18" s="21">
         <v>3</v>
@@ -1662,13 +1667,13 @@
         <v>15</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" s="30">
         <v>9</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L19" s="21">
         <v>3</v>
@@ -1680,23 +1685,23 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="16"/>
       <c r="F20" s="4">
         <v>16</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="30">
         <v>11</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L20" s="21">
         <v>3</v>
@@ -1711,20 +1716,20 @@
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D21" s="16"/>
       <c r="F21" s="4">
         <v>17</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H21" s="30">
         <v>8</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L21" s="21">
         <v>3</v>
@@ -1739,20 +1744,20 @@
         <v>2</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="16"/>
       <c r="F22" s="4">
         <v>18</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="30">
         <v>12</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L22" s="21">
         <v>3</v>
@@ -1767,20 +1772,20 @@
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="16"/>
       <c r="F23" s="4">
         <v>19</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="30">
         <v>13</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L23" s="21">
         <v>4</v>
@@ -1795,20 +1800,20 @@
         <v>4</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24" s="16"/>
       <c r="F24" s="4">
         <v>20</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H24" s="30">
         <v>4</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L24" s="21">
         <v>4</v>
@@ -1823,20 +1828,20 @@
         <v>5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25" s="16"/>
       <c r="F25" s="4">
         <v>21</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="30">
         <v>1</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L25" s="21">
         <v>4</v>
@@ -1851,20 +1856,20 @@
         <v>6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="16"/>
       <c r="F26" s="4">
         <v>22</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="30">
         <v>8</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L26" s="21">
         <v>4</v>
@@ -1879,20 +1884,20 @@
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D27" s="16"/>
       <c r="F27" s="4">
         <v>23</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" s="30">
         <v>14</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L27" s="21">
         <v>5</v>
@@ -1907,20 +1912,20 @@
         <v>8</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28" s="16"/>
       <c r="F28" s="4">
         <v>24</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="30">
         <v>15</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L28" s="21">
         <v>5</v>
@@ -1935,20 +1940,20 @@
         <v>9</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29" s="16"/>
       <c r="F29" s="4">
         <v>25</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H29" s="30">
         <v>10</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L29" s="21">
         <v>5</v>
@@ -1963,20 +1968,20 @@
         <v>10</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D30" s="16"/>
       <c r="F30" s="4">
         <v>26</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H30" s="30">
         <v>17</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L30" s="21">
         <v>5</v>
@@ -1991,20 +1996,20 @@
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D31" s="16"/>
       <c r="F31" s="4">
         <v>27</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H31" s="30">
         <v>16</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L31" s="21">
         <v>6</v>
@@ -2019,20 +2024,20 @@
         <v>12</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D32" s="16"/>
       <c r="F32" s="4">
         <v>28</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H32" s="33">
         <v>18</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L32" s="21">
         <v>6</v>
@@ -2047,20 +2052,20 @@
         <v>13</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D33" s="16"/>
       <c r="F33" s="4">
         <v>29</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H33" s="33">
         <v>10</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L33" s="21">
         <v>6</v>
@@ -2075,20 +2080,20 @@
         <v>14</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D34" s="16"/>
       <c r="F34" s="4">
         <v>30</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" s="30">
         <v>7</v>
       </c>
       <c r="I34" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L34" s="21">
         <v>6</v>
@@ -2103,20 +2108,20 @@
         <v>15</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D35" s="16"/>
       <c r="F35" s="6">
         <v>31</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" s="34">
         <v>3</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L35" s="21">
         <v>4</v>
@@ -2131,7 +2136,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36" s="16"/>
       <c r="L36" s="21">
@@ -2147,7 +2152,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D37" s="16"/>
       <c r="L37" s="21">
@@ -2163,7 +2168,7 @@
         <v>18</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D38" s="11"/>
       <c r="L38" s="21">
@@ -2189,7 +2194,7 @@
     </row>
     <row r="41" spans="2:14" ht="18">
       <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="29"/>
@@ -2203,13 +2208,13 @@
     </row>
     <row r="43" spans="2:14">
       <c r="B43" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E43" s="37"/>
     </row>
@@ -2218,10 +2223,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E44" s="37"/>
     </row>
@@ -2230,10 +2235,10 @@
         <v>2</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E45" s="37"/>
     </row>
@@ -2242,10 +2247,10 @@
         <v>3</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E46" s="37"/>
     </row>
@@ -2254,10 +2259,10 @@
         <v>4</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E47" s="37"/>
     </row>
@@ -2266,10 +2271,10 @@
         <v>5</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E48" s="37"/>
     </row>
@@ -2278,10 +2283,10 @@
         <v>6</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E49" s="37"/>
     </row>
@@ -2290,10 +2295,10 @@
         <v>7</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E50" s="37"/>
     </row>
@@ -2302,10 +2307,10 @@
         <v>8</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E51" s="37"/>
     </row>
@@ -2314,10 +2319,10 @@
         <v>9</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E52" s="37"/>
     </row>
@@ -2326,10 +2331,10 @@
         <v>10</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E53" s="37"/>
     </row>
@@ -2338,10 +2343,10 @@
         <v>11</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E54" s="37"/>
     </row>
@@ -2350,10 +2355,10 @@
         <v>12</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E55" s="37"/>
     </row>

</xml_diff>